<commit_message>
[IMP] Stable version 20230113
</commit_message>
<xml_diff>
--- a/tools/odoo_template_tnl.xlsx
+++ b/tools/odoo_template_tnl.xlsx
@@ -23092,7 +23092,7 @@
     <t xml:space="preserve">Set your company's data for documents header/footer</t>
   </si>
   <si>
-    <t xml:space="preserve">Imposta le informazioni aziendali per l'intestazione/piè di pagina dei documenti</t>
+    <t xml:space="preserve">Impostare i dati aziendali per l'intestazione/piè di pagina dei documenti</t>
   </si>
   <si>
     <t xml:space="preserve">Setting</t>
@@ -28277,7 +28277,7 @@
     <t xml:space="preserve">Your company %s is not set</t>
   </si>
   <si>
-    <t xml:space="preserve">%s azienda non impostato/a</t>
+    <t xml:space="preserve">Azienda %s non impostato/a</t>
   </si>
   <si>
     <t xml:space="preserve">Your company City is not set</t>
@@ -28471,15 +28471,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="00FFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
 </styleSheet>
 </file>
 
@@ -28490,8 +28481,8 @@
   </sheetPr>
   <dimension ref="A1:C4712"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4699" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4479" activeCellId="0" sqref="A4479"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3778" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3787" activeCellId="0" sqref="C3787"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.07421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>